<commit_message>
FINAL PRODUCT FROM ANNA: merge these files into master please!Except for ClassRoom.xlsx, thats the old one
</commit_message>
<xml_diff>
--- a/PythonScheduler/ClassRoom_extra2.xlsx
+++ b/PythonScheduler/ClassRoom_extra2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayajae/Desktop/447Proj-anna_branch/PythonScheduler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parul\Desktop\UMBC\semester 8\447\Project\GitV\PythonScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD987D1-274F-44CD-B8F5-160270918557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2840" windowWidth="19040" windowHeight="13820" activeTab="2"/>
+    <workbookView xWindow="2235" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -21,18 +22,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="155">
   <si>
     <t>Subject</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Discrete Structures</t>
   </si>
   <si>
-    <t xml:space="preserve">CMSC </t>
-  </si>
-  <si>
     <t>Continued Computer Science for Non-Majors</t>
   </si>
   <si>
@@ -455,12 +453,57 @@
   </si>
   <si>
     <t xml:space="preserve">University Center </t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>BIOL</t>
+  </si>
+  <si>
+    <t>CMPE</t>
+  </si>
+  <si>
+    <t>HIST</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>BTEC</t>
+  </si>
+  <si>
+    <t>PYSC</t>
+  </si>
+  <si>
+    <t>CHEM</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>POLI</t>
+  </si>
+  <si>
+    <t>STAT</t>
+  </si>
+  <si>
+    <t>ECON</t>
+  </si>
+  <si>
+    <t>ENGL</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -586,6 +629,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,27 +914,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1" hidden="1"/>
+    <col min="1" max="1" width="10.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="10.85546875" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -913,10 +957,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -930,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>9</v>
@@ -939,7 +983,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -953,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>10</v>
@@ -962,7 +1006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -976,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>9</v>
@@ -985,7 +1029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>13</v>
@@ -1008,7 +1052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>14</v>
@@ -1031,7 +1075,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>15</v>
@@ -1054,7 +1098,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>16</v>
@@ -1077,7 +1121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>18</v>
@@ -1100,7 +1144,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>10</v>
@@ -1123,7 +1167,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>19</v>
@@ -1146,7 +1190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
@@ -1160,7 +1204,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>20</v>
@@ -1169,7 +1213,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1227,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>14</v>
@@ -1192,7 +1236,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -1206,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>9</v>
@@ -1215,7 +1259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>9</v>
@@ -1238,7 +1282,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>10</v>
@@ -1261,7 +1305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -1275,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>18</v>
@@ -1284,7 +1328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +1342,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>15</v>
@@ -1307,7 +1351,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
@@ -1321,7 +1365,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>14</v>
@@ -1330,7 +1374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>13</v>
@@ -1353,30 +1397,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B21" s="9">
         <v>291</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="E21" s="10">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="H21" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -1384,14 +1428,14 @@
         <v>304</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="10">
         <v>1</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>9</v>
@@ -1400,7 +1444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -1408,13 +1452,13 @@
         <v>304</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="10">
         <v>2</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>9</v>
@@ -1423,7 +1467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
@@ -1431,22 +1475,22 @@
         <v>304</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="10">
         <v>3</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
@@ -1454,13 +1498,13 @@
         <v>304</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="10">
         <v>4</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>10</v>
@@ -1469,7 +1513,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -1477,22 +1521,22 @@
         <v>304</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="10">
         <v>5</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H26" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -1500,13 +1544,13 @@
         <v>304</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="10">
         <v>6</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>9</v>
@@ -1515,7 +1559,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -1523,13 +1567,13 @@
         <v>304</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="10">
         <v>7</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>10</v>
@@ -1538,7 +1582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
@@ -1546,13 +1590,13 @@
         <v>313</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" s="10">
         <v>1</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>15</v>
@@ -1561,7 +1605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>7</v>
       </c>
@@ -1569,13 +1613,13 @@
         <v>313</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="10">
         <v>2</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>20</v>
@@ -1584,7 +1628,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1592,13 +1636,13 @@
         <v>313</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" s="10">
         <v>3</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>14</v>
@@ -1607,7 +1651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>7</v>
       </c>
@@ -1615,13 +1659,13 @@
         <v>313</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" s="10">
         <v>4</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>13</v>
@@ -1630,7 +1674,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>7</v>
       </c>
@@ -1638,13 +1682,13 @@
         <v>331</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="10">
         <v>1</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>18</v>
@@ -1653,7 +1697,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>7</v>
       </c>
@@ -1661,22 +1705,22 @@
         <v>331</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="10">
         <v>2</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H34" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>7</v>
       </c>
@@ -1684,13 +1728,13 @@
         <v>331</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" s="10">
         <v>3</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>14</v>
@@ -1699,7 +1743,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>7</v>
       </c>
@@ -1707,13 +1751,13 @@
         <v>331</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="10">
         <v>4</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>20</v>
@@ -1722,7 +1766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>7</v>
       </c>
@@ -1730,22 +1774,22 @@
         <v>341</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="10">
         <v>1</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H37" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>7</v>
       </c>
@@ -1753,22 +1797,22 @@
         <v>341</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" s="10">
         <v>2</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H38" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>7</v>
       </c>
@@ -1776,13 +1820,13 @@
         <v>341</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" s="10">
         <v>3</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>19</v>
@@ -1791,7 +1835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>7</v>
       </c>
@@ -1799,13 +1843,13 @@
         <v>341</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E40" s="10">
         <v>4</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>14</v>
@@ -1814,7 +1858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>7</v>
       </c>
@@ -1822,13 +1866,13 @@
         <v>341</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" s="10">
         <v>5</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>13</v>
@@ -1837,7 +1881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>7</v>
       </c>
@@ -1845,13 +1889,13 @@
         <v>341</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42" s="10">
         <v>6</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>16</v>
@@ -1860,21 +1904,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="E43" s="10">
         <v>1</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>19</v>
@@ -1883,21 +1927,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>14</v>
@@ -1906,21 +1950,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="10">
         <v>2</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>13</v>
@@ -1929,21 +1973,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" s="10">
         <v>3</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>9</v>
@@ -1952,7 +1996,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>7</v>
       </c>
@@ -1960,13 +2004,13 @@
         <v>421</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="10">
         <v>1</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>15</v>
@@ -1975,7 +2019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>7</v>
       </c>
@@ -1983,13 +2027,13 @@
         <v>421</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="10">
         <v>2</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>19</v>
@@ -1998,7 +2042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
@@ -2006,13 +2050,13 @@
         <v>421</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="10">
         <v>3</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>10</v>
@@ -2021,7 +2065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>7</v>
       </c>
@@ -2029,22 +2073,22 @@
         <v>426</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E50" s="10">
         <v>1</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H50" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>7</v>
       </c>
@@ -2052,13 +2096,13 @@
         <v>426</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E51" s="10">
         <v>3</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>20</v>
@@ -2067,21 +2111,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="E52" s="10">
         <v>1</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>14</v>
@@ -2090,7 +2134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>7</v>
       </c>
@@ -2098,22 +2142,22 @@
         <v>441</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E53" s="10">
         <v>1</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H53" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>7</v>
       </c>
@@ -2121,13 +2165,13 @@
         <v>441</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E54" s="10">
         <v>2</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>18</v>
@@ -2136,7 +2180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>7</v>
       </c>
@@ -2144,36 +2188,36 @@
         <v>441</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E55" s="10">
         <v>3</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H55" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="10">
         <v>1</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>18</v>
@@ -2182,7 +2226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>7</v>
       </c>
@@ -2190,13 +2234,13 @@
         <v>447</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E57" s="10">
         <v>1</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>14</v>
@@ -2205,7 +2249,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>7</v>
       </c>
@@ -2213,13 +2257,13 @@
         <v>447</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E58" s="10">
         <v>2</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>13</v>
@@ -2228,7 +2272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>7</v>
       </c>
@@ -2236,13 +2280,13 @@
         <v>447</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E59" s="10">
         <v>3</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>9</v>
@@ -2251,7 +2295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>7</v>
       </c>
@@ -2259,22 +2303,22 @@
         <v>447</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E60" s="10">
         <v>4</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H60" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>7</v>
       </c>
@@ -2282,13 +2326,13 @@
         <v>455</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E61" s="10">
         <v>2</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>16</v>
@@ -2297,7 +2341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>7</v>
       </c>
@@ -2305,13 +2349,13 @@
         <v>461</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E62" s="10">
         <v>1</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>15</v>
@@ -2320,7 +2364,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>7</v>
       </c>
@@ -2328,13 +2372,13 @@
         <v>461</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E63" s="10">
         <v>2</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>13</v>
@@ -2343,7 +2387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>7</v>
       </c>
@@ -2351,13 +2395,13 @@
         <v>471</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E64" s="10">
         <v>1</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>16</v>
@@ -2366,7 +2410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>7</v>
       </c>
@@ -2374,13 +2418,13 @@
         <v>471</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E65" s="10">
         <v>2</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>20</v>
@@ -2389,7 +2433,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>7</v>
       </c>
@@ -2397,13 +2441,13 @@
         <v>471</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E66" s="10">
         <v>3</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>10</v>
@@ -2412,21 +2456,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="E67" s="10">
         <v>1</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>14</v>
@@ -2435,7 +2479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>7</v>
       </c>
@@ -2443,13 +2487,13 @@
         <v>478</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E68" s="10">
         <v>1</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>9</v>
@@ -2458,7 +2502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>7</v>
       </c>
@@ -2466,13 +2510,13 @@
         <v>478</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E69" s="10">
         <v>2</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>15</v>
@@ -2481,21 +2525,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="E70" s="10">
         <v>1</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>19</v>
@@ -2504,7 +2548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>7</v>
       </c>
@@ -2512,13 +2556,13 @@
         <v>481</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E71" s="10">
         <v>1</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>20</v>
@@ -2527,7 +2571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>7</v>
       </c>
@@ -2535,36 +2579,36 @@
         <v>691</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E72" s="10">
         <v>1</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H72" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="E73" s="10">
         <v>1</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>9</v>
@@ -2573,47 +2617,47 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B74" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="E74" s="10">
         <v>1</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H74" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="D75" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="E75" s="10">
         <v>1</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>10</v>
@@ -2622,24 +2666,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C76" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="E76" s="10">
         <v>1</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>20</v>
@@ -2648,7 +2692,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>7</v>
       </c>
@@ -2656,16 +2700,16 @@
         <v>491</v>
       </c>
       <c r="C77" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="E77" s="10">
         <v>1</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>16</v>
@@ -2674,7 +2718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>7</v>
       </c>
@@ -2682,22 +2726,22 @@
         <v>493</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E78" s="10">
         <v>1</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H78" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>7</v>
       </c>
@@ -2705,13 +2749,13 @@
         <v>611</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E79" s="10">
         <v>1</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>20</v>
@@ -2720,7 +2764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>7</v>
       </c>
@@ -2728,13 +2772,13 @@
         <v>611</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E80" s="10">
         <v>2</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>9</v>
@@ -2743,7 +2787,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>7</v>
       </c>
@@ -2751,22 +2795,22 @@
         <v>621</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E81" s="10">
         <v>1</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H81" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>7</v>
       </c>
@@ -2774,22 +2818,22 @@
         <v>641</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E82" s="10">
         <v>1</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H82" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>7</v>
       </c>
@@ -2797,13 +2841,13 @@
         <v>678</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E83" s="10">
         <v>1</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>19</v>
@@ -2812,7 +2856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>7</v>
       </c>
@@ -2820,14 +2864,14 @@
         <v>682</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="10">
         <v>1</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>9</v>
@@ -2836,7 +2880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>7</v>
       </c>
@@ -2844,13 +2888,13 @@
         <v>682</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E85" s="10">
         <v>2</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>9</v>
@@ -2859,7 +2903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>7</v>
       </c>
@@ -2867,22 +2911,22 @@
         <v>684</v>
       </c>
       <c r="C86" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E86" s="10">
+        <v>1</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G86" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E86" s="10">
-        <v>1</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="H86" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>7</v>
       </c>
@@ -2890,13 +2934,13 @@
         <v>684</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E87" s="10">
         <v>2</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>9</v>
@@ -2905,7 +2949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>7</v>
       </c>
@@ -2913,16 +2957,16 @@
         <v>691</v>
       </c>
       <c r="C88" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="E88" s="10">
         <v>1</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>16</v>
@@ -2931,24 +2975,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>14</v>
@@ -2957,21 +3001,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E90" s="10">
         <v>1</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G90" s="10" t="s">
         <v>9</v>
@@ -2980,148 +3024,148 @@
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" hidden="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="A2:B17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition descending="1" ref="B2:B17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3129,34 +3173,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="B2" s="13">
         <v>39.253003999999997</v>
@@ -3164,10 +3211,13 @@
       <c r="C2" s="13">
         <v>-76.713624999999993</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="13">
         <v>39.256816999999998</v>
@@ -3175,10 +3225,13 @@
       <c r="C3" s="13">
         <v>-76.711589000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="13">
         <v>39.255226</v>
@@ -3186,10 +3239,13 @@
       <c r="C4" s="13">
         <v>-76.715367000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="13">
         <v>39.254835999999997</v>
@@ -3197,10 +3253,13 @@
       <c r="C5" s="13">
         <v>-76.712238999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="13">
         <v>39.254564000000002</v>
@@ -3208,10 +3267,13 @@
       <c r="C6" s="13">
         <v>-76.714027000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="13">
         <v>39.255181999999998</v>
@@ -3219,10 +3281,13 @@
       <c r="C7" s="13">
         <v>-76.713509999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="13">
         <v>39.253858999999999</v>
@@ -3230,10 +3295,13 @@
       <c r="C8" s="13">
         <v>-76.714301000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="13">
         <v>39.253901999999997</v>
@@ -3241,10 +3309,13 @@
       <c r="C9" s="13">
         <v>-76.710881000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="13">
         <v>39.253492999999999</v>
@@ -3252,10 +3323,13 @@
       <c r="C10" s="13">
         <v>-76.712834000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="13">
         <v>39.254826999999999</v>
@@ -3263,10 +3337,13 @@
       <c r="C11" s="13">
         <v>-76.711819000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="13">
         <v>39.254106</v>
@@ -3274,10 +3351,13 @@
       <c r="C12" s="13">
         <v>-76.712485999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="13">
         <v>39.255065000000002</v>
@@ -3285,10 +3365,13 @@
       <c r="C13" s="13">
         <v>-76.713108000000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="13">
         <v>39.254519000000002</v>
@@ -3296,10 +3379,13 @@
       <c r="C14" s="13">
         <v>-76.709598999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="13">
         <v>39.255243</v>
@@ -3307,10 +3393,13 @@
       <c r="C15" s="13">
         <v>-76.709035</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" s="13">
         <v>39.253579999999999</v>
@@ -3318,10 +3407,13 @@
       <c r="C16" s="13">
         <v>-76.713229999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="13">
         <v>39.254387999999999</v>
@@ -3329,13 +3421,17 @@
       <c r="C17" s="13">
         <v>-76.713317000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>